<commit_message>
Add warnings and more motor related logic
</commit_message>
<xml_diff>
--- a/Motor_data.xlsx
+++ b/Motor_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janni\Desktop\KBE_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9ED359-E793-4815-A1BD-1DDECAE0CD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09533C0A-D7FF-4F0E-9510-35F2CF94E0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>kV (RPM/V)</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>SunnySky X Series V3 X2220 KV2200</t>
+  </si>
+  <si>
+    <t>SunnySky X Series V3 X2305 KV1450</t>
   </si>
 </sst>
 </file>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,6 +668,32 @@
         <v>85</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>1450</v>
+      </c>
+      <c r="C11">
+        <v>0.12</v>
+      </c>
+      <c r="D11">
+        <v>20.5</v>
+      </c>
+      <c r="E11">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>12.6</v>
+      </c>
+      <c r="H11">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>